<commit_message>
added sample_period. seems like that change was made before, but didn't get committed.
</commit_message>
<xml_diff>
--- a/sb3002 data/super_pot/super_pot_TE_DataEntryForm.xlsx
+++ b/sb3002 data/super_pot/super_pot_TE_DataEntryForm.xlsx
@@ -1380,6 +1380,15 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1396,15 +1405,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1724,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,11 +1770,11 @@
       <c r="B2" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
       <c r="H2" s="47"/>
       <c r="I2" s="95" t="s">
         <v>152</v>
@@ -1796,11 +1796,11 @@
       <c r="B3" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
       <c r="H3" s="47"/>
       <c r="I3" s="98"/>
       <c r="J3" s="91"/>
@@ -1820,11 +1820,11 @@
       <c r="B4" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
       <c r="H4" s="47"/>
       <c r="I4" s="98"/>
       <c r="J4" s="91"/>
@@ -1844,11 +1844,11 @@
       <c r="B5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="122"/>
       <c r="H5" s="47"/>
       <c r="I5" s="69"/>
       <c r="J5" s="91"/>
@@ -1868,11 +1868,11 @@
       <c r="B6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
       <c r="H6" s="47"/>
       <c r="I6" s="106" t="s">
         <v>153</v>
@@ -1894,11 +1894,11 @@
       <c r="B7" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
       <c r="H7" s="47"/>
       <c r="I7" s="98"/>
       <c r="J7" s="91"/>
@@ -2315,14 +2315,14 @@
         <v>131</v>
       </c>
       <c r="C22" s="58"/>
-      <c r="D22" s="126" t="s">
+      <c r="D22" s="120" t="s">
         <v>134</v>
       </c>
-      <c r="E22" s="127"/>
-      <c r="F22" s="126" t="s">
+      <c r="E22" s="121"/>
+      <c r="F22" s="120" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="127"/>
+      <c r="G22" s="121"/>
       <c r="H22" s="47"/>
       <c r="I22" s="65"/>
       <c r="J22" s="93"/>
@@ -2557,28 +2557,28 @@
         <v>3</v>
       </c>
       <c r="E30" s="18"/>
-      <c r="F30" s="120" t="s">
+      <c r="F30" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="121"/>
+      <c r="G30" s="124"/>
       <c r="H30" s="4"/>
       <c r="I30" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J30" s="7"/>
-      <c r="K30" s="120" t="s">
+      <c r="K30" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="L30" s="121"/>
+      <c r="L30" s="124"/>
       <c r="M30" s="4"/>
       <c r="N30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="O30" s="18"/>
-      <c r="P30" s="120" t="s">
+      <c r="P30" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="Q30" s="124"/>
+      <c r="Q30" s="127"/>
       <c r="R30" s="47"/>
       <c r="S30" s="47"/>
       <c r="T30" s="47"/>
@@ -2589,24 +2589,24 @@
       <c r="C31" s="5"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="122" t="s">
+      <c r="F31" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="123"/>
+      <c r="G31" s="126"/>
       <c r="H31" s="4"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="122" t="s">
+      <c r="K31" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="123"/>
+      <c r="L31" s="126"/>
       <c r="M31" s="4"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
-      <c r="P31" s="122" t="s">
+      <c r="P31" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="Q31" s="125"/>
+      <c r="Q31" s="128"/>
       <c r="R31" s="47"/>
       <c r="S31" s="47"/>
       <c r="T31" s="47"/>
@@ -3216,21 +3216,27 @@
       <c r="C46" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="109"/>
+      <c r="D46" s="109">
+        <v>98.7</v>
+      </c>
       <c r="E46" s="71" t="s">
         <v>71</v>
       </c>
       <c r="F46" s="85"/>
       <c r="G46" s="86"/>
       <c r="H46" s="63"/>
-      <c r="I46" s="109"/>
+      <c r="I46" s="109">
+        <v>98.6</v>
+      </c>
       <c r="J46" s="71" t="s">
         <v>97</v>
       </c>
       <c r="K46" s="85"/>
       <c r="L46" s="86"/>
       <c r="M46" s="63"/>
-      <c r="N46" s="109"/>
+      <c r="N46" s="109">
+        <v>96.4</v>
+      </c>
       <c r="O46" s="71" t="s">
         <v>123</v>
       </c>
@@ -4434,6 +4440,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="P31:Q31"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="C2:G2"/>
@@ -4442,12 +4454,6 @@
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="P31:Q31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>